<commit_message>
Update TrackList.xlsx & move wireframes
</commit_message>
<xml_diff>
--- a/TrackList.xlsx
+++ b/TrackList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Team-Code_Life\mefado-ui-design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9907E1BB-891A-48FC-B51A-E890356C5093}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E884F5C9-5141-4639-A05B-09D9E825EE7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{279BB581-13DC-4C67-A208-ECEAEC5F3134}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="114">
   <si>
     <t>Outcomes</t>
   </si>
@@ -309,33 +309,6 @@
     <t>OUT04-02-M</t>
   </si>
   <si>
-    <t>OUT01-01-D</t>
-  </si>
-  <si>
-    <t>OUT01-02-D</t>
-  </si>
-  <si>
-    <t>OUT02-02-D</t>
-  </si>
-  <si>
-    <t>OUT02-01-D</t>
-  </si>
-  <si>
-    <t>OUT03-02-D</t>
-  </si>
-  <si>
-    <t>OUT03-01-D</t>
-  </si>
-  <si>
-    <t>OUT04-01-D</t>
-  </si>
-  <si>
-    <t>OUT04-02-D</t>
-  </si>
-  <si>
-    <t>OUT05-01-D</t>
-  </si>
-  <si>
     <t>OUT05-01-M</t>
   </si>
   <si>
@@ -354,24 +327,9 @@
     <t>EXT01-05-M</t>
   </si>
   <si>
-    <t>EXT01-01-D</t>
-  </si>
-  <si>
-    <t>EXT01-04-D</t>
-  </si>
-  <si>
-    <t>EXT01-03-D</t>
-  </si>
-  <si>
-    <t>EXT01-02-D</t>
-  </si>
-  <si>
     <t>OUT06-01-M</t>
   </si>
   <si>
-    <t>OUT06-01-D</t>
-  </si>
-  <si>
     <t>OUT07-01-M</t>
   </si>
   <si>
@@ -423,61 +381,22 @@
     <t>OUT09-03-M</t>
   </si>
   <si>
-    <t>OUT07-01-D</t>
-  </si>
-  <si>
-    <t>OUT07-02-D</t>
-  </si>
-  <si>
-    <t>OUT07-03-D</t>
-  </si>
-  <si>
-    <t>OUT07-04-D</t>
-  </si>
-  <si>
-    <t>OUT07-05-D</t>
-  </si>
-  <si>
-    <t>OUT07-06-D</t>
-  </si>
-  <si>
-    <t>OUT07-07-D</t>
-  </si>
-  <si>
-    <t>OUT07-08-D</t>
-  </si>
-  <si>
-    <t>OUT07-09-D</t>
-  </si>
-  <si>
-    <t>OUT07-10-D</t>
-  </si>
-  <si>
-    <t>OUT07-11-D</t>
-  </si>
-  <si>
-    <t>OUT07-12-D</t>
-  </si>
-  <si>
-    <t>OUT08-01-D</t>
-  </si>
-  <si>
-    <t>OUT08-02-D</t>
-  </si>
-  <si>
-    <t>OUT09-01-D</t>
-  </si>
-  <si>
-    <t>OUT09-02-D</t>
-  </si>
-  <si>
-    <t>OUT09-03-D</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
     <t>EXT01</t>
+  </si>
+  <si>
+    <t>EXT01-06-M</t>
+  </si>
+  <si>
+    <t>Sửa thông tin bộ sưu tập</t>
+  </si>
+  <si>
+    <t>Xem DS các bài đăng (list view)</t>
+  </si>
+  <si>
+    <t>Xem DS các bài đăng (map view)</t>
   </si>
 </sst>
 </file>
@@ -745,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -926,9 +845,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2063,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95DB2D2-227C-4DF4-891D-B90556287239}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2195,19 +2111,17 @@
         <v>76</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="I4" s="32"/>
       <c r="J4" s="32" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="K4" s="32"/>
       <c r="L4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="9" t="s">
-        <v>84</v>
-      </c>
+      <c r="M4" s="9"/>
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
       <c r="P4" s="32"/>
@@ -2227,19 +2141,17 @@
         <v>77</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="I5" s="31"/>
       <c r="J5" s="31" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="K5" s="31"/>
       <c r="L5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="M5" s="11"/>
       <c r="N5" s="31"/>
       <c r="O5" s="31"/>
       <c r="P5" s="31"/>
@@ -2267,19 +2179,17 @@
         <v>78</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="30" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="K6" s="30"/>
       <c r="L6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="13" t="s">
-        <v>87</v>
-      </c>
+      <c r="M6" s="13"/>
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2299,19 +2209,17 @@
         <v>79</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="I7" s="31"/>
       <c r="J7" s="31" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="K7" s="31"/>
       <c r="L7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M7" s="11" t="s">
-        <v>86</v>
-      </c>
+      <c r="M7" s="11"/>
       <c r="N7" s="31"/>
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
@@ -2340,14 +2248,14 @@
       </c>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
+      <c r="J8" s="27" t="s">
+        <v>108</v>
+      </c>
       <c r="K8" s="27"/>
       <c r="L8" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="M8" s="13" t="s">
-        <v>89</v>
-      </c>
+      <c r="M8" s="13"/>
       <c r="N8" s="27"/>
       <c r="O8" s="27" t="s">
         <v>9</v>
@@ -2369,14 +2277,14 @@
       </c>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
+      <c r="J9" s="29" t="s">
+        <v>108</v>
+      </c>
       <c r="K9" s="29"/>
       <c r="L9" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>88</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="M9" s="11"/>
       <c r="N9" s="29"/>
       <c r="O9" s="29"/>
       <c r="P9" s="29"/>
@@ -2405,7 +2313,7 @@
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="K10" s="27" t="s">
         <v>10</v>
@@ -2413,9 +2321,7 @@
       <c r="L10" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="M10" s="13" t="s">
-        <v>90</v>
-      </c>
+      <c r="M10" s="13"/>
       <c r="N10" s="27"/>
       <c r="O10" s="27"/>
       <c r="P10" s="27"/>
@@ -2437,14 +2343,14 @@
       </c>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
+      <c r="J11" s="29" t="s">
+        <v>108</v>
+      </c>
       <c r="K11" s="29"/>
       <c r="L11" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="M11" s="11" t="s">
-        <v>91</v>
-      </c>
+      <c r="M11" s="11"/>
       <c r="N11" s="29"/>
       <c r="O11" s="29"/>
       <c r="P11" s="29"/>
@@ -2468,18 +2374,18 @@
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="22" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
+      <c r="J12" s="26" t="s">
+        <v>108</v>
+      </c>
       <c r="K12" s="26"/>
       <c r="L12" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="M12" s="22" t="s">
-        <v>92</v>
-      </c>
+      <c r="M12" s="22"/>
       <c r="N12" s="26"/>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -2490,7 +2396,7 @@
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="35" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>58</v>
@@ -2503,7 +2409,7 @@
       </c>
       <c r="F13" s="41"/>
       <c r="G13" s="15" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="H13" s="27" t="s">
         <v>27</v>
@@ -2512,15 +2418,13 @@
         <v>27</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="K13" s="27"/>
       <c r="L13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="15" t="s">
-        <v>99</v>
-      </c>
+      <c r="M13" s="1"/>
       <c r="N13" s="27" t="s">
         <v>27</v>
       </c>
@@ -2541,7 +2445,7 @@
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
       <c r="G14" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H14" s="28" t="s">
         <v>27</v>
@@ -2550,14 +2454,11 @@
         <v>27</v>
       </c>
       <c r="J14" s="28" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="K14" s="28"/>
       <c r="L14" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="N14" s="28" t="s">
         <v>27</v>
@@ -2582,7 +2483,7 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H15" s="28" t="s">
         <v>27</v>
@@ -2591,15 +2492,13 @@
         <v>27</v>
       </c>
       <c r="J15" s="28" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="K15" s="28"/>
       <c r="L15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="M15" s="1"/>
       <c r="N15" s="28" t="s">
         <v>27</v>
       </c>
@@ -2623,7 +2522,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H16" s="28" t="s">
         <v>27</v>
@@ -2631,19 +2530,18 @@
       <c r="I16" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="28"/>
+      <c r="J16" s="28" t="s">
+        <v>108</v>
+      </c>
       <c r="K16" s="28"/>
       <c r="L16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M16" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="61"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B17" s="36"/>
@@ -2656,7 +2554,7 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H17" s="28" t="s">
         <v>27</v>
@@ -2667,11 +2565,9 @@
       <c r="J17" s="28"/>
       <c r="K17" s="28"/>
       <c r="L17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>100</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="M17" s="1"/>
       <c r="N17" s="28" t="s">
         <v>27</v>
       </c>
@@ -2694,7 +2590,9 @@
         <v>27</v>
       </c>
       <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="H18" s="29" t="s">
         <v>27</v>
       </c>
@@ -2703,7 +2601,9 @@
       </c>
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
-      <c r="L18" s="17"/>
+      <c r="L18" s="17" t="s">
+        <v>111</v>
+      </c>
       <c r="M18" s="17"/>
       <c r="N18" s="29" t="s">
         <v>27</v>
@@ -2733,7 +2633,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="H19" s="26" t="s">
         <v>27</v>
@@ -2746,9 +2646,7 @@
       <c r="L19" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="M19" s="22" t="s">
-        <v>104</v>
-      </c>
+      <c r="M19" s="22"/>
       <c r="N19" s="26" t="s">
         <v>27</v>
       </c>
@@ -2777,7 +2675,7 @@
       </c>
       <c r="F20" s="38"/>
       <c r="G20" s="15" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="H20" s="27" t="s">
         <v>27</v>
@@ -2790,9 +2688,7 @@
       <c r="L20" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="M20" s="15" t="s">
-        <v>122</v>
-      </c>
+      <c r="M20" s="15"/>
       <c r="N20" s="27" t="s">
         <v>27</v>
       </c>
@@ -2813,7 +2709,7 @@
       <c r="E21" s="42"/>
       <c r="F21" s="39"/>
       <c r="G21" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="H21" s="28" t="s">
         <v>27</v>
@@ -2826,9 +2722,7 @@
       <c r="L21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="M21" s="1"/>
       <c r="N21" s="28" t="s">
         <v>27</v>
       </c>
@@ -2849,7 +2743,7 @@
       <c r="E22" s="42"/>
       <c r="F22" s="39"/>
       <c r="G22" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="H22" s="28" t="s">
         <v>27</v>
@@ -2862,9 +2756,7 @@
       <c r="L22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>124</v>
-      </c>
+      <c r="M22" s="1"/>
       <c r="N22" s="28" t="s">
         <v>27</v>
       </c>
@@ -2885,7 +2777,7 @@
       <c r="E23" s="42"/>
       <c r="F23" s="39"/>
       <c r="G23" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="H23" s="28" t="s">
         <v>27</v>
@@ -2898,9 +2790,7 @@
       <c r="L23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="M23" s="1"/>
       <c r="N23" s="28" t="s">
         <v>27</v>
       </c>
@@ -2921,7 +2811,7 @@
       <c r="E24" s="42"/>
       <c r="F24" s="39"/>
       <c r="G24" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="H24" s="28" t="s">
         <v>27</v>
@@ -2934,9 +2824,7 @@
       <c r="L24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="M24" s="1"/>
       <c r="N24" s="28" t="s">
         <v>27</v>
       </c>
@@ -2956,7 +2844,7 @@
       <c r="E25" s="42"/>
       <c r="F25" s="39"/>
       <c r="G25" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="H25" s="28" t="s">
         <v>27</v>
@@ -2969,9 +2857,7 @@
       <c r="L25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="M25" s="1"/>
       <c r="N25" s="28" t="s">
         <v>27</v>
       </c>
@@ -2992,7 +2878,7 @@
       <c r="E26" s="42"/>
       <c r="F26" s="39"/>
       <c r="G26" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="H26" s="28" t="s">
         <v>27</v>
@@ -3005,9 +2891,7 @@
       <c r="L26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="M26" s="1"/>
       <c r="N26" s="28" t="s">
         <v>27</v>
       </c>
@@ -3027,7 +2911,7 @@
       <c r="E27" s="42"/>
       <c r="F27" s="39"/>
       <c r="G27" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="H27" s="28" t="s">
         <v>27</v>
@@ -3040,9 +2924,7 @@
       <c r="L27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="M27" s="1"/>
       <c r="N27" s="28" t="s">
         <v>27</v>
       </c>
@@ -3062,7 +2944,7 @@
       <c r="E28" s="42"/>
       <c r="F28" s="39"/>
       <c r="G28" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="H28" s="28" t="s">
         <v>27</v>
@@ -3075,9 +2957,7 @@
       <c r="L28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="M28" s="1"/>
       <c r="N28" s="28" t="s">
         <v>27</v>
       </c>
@@ -3097,7 +2977,7 @@
       <c r="E29" s="42"/>
       <c r="F29" s="39"/>
       <c r="G29" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="H29" s="28" t="s">
         <v>27</v>
@@ -3110,9 +2990,7 @@
       <c r="L29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="M29" s="1"/>
       <c r="N29" s="28" t="s">
         <v>27</v>
       </c>
@@ -3132,7 +3010,7 @@
       <c r="E30" s="42"/>
       <c r="F30" s="39"/>
       <c r="G30" s="1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="H30" s="28" t="s">
         <v>27</v>
@@ -3145,9 +3023,7 @@
       <c r="L30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M30" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="M30" s="1"/>
       <c r="N30" s="28" t="s">
         <v>27</v>
       </c>
@@ -3167,7 +3043,7 @@
       <c r="E31" s="43"/>
       <c r="F31" s="40"/>
       <c r="G31" s="17" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="H31" s="29" t="s">
         <v>27</v>
@@ -3180,9 +3056,7 @@
       <c r="L31" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M31" s="17" t="s">
-        <v>133</v>
-      </c>
+      <c r="M31" s="17"/>
       <c r="N31" s="29" t="s">
         <v>27</v>
       </c>
@@ -3210,7 +3084,7 @@
       </c>
       <c r="F32" s="41"/>
       <c r="G32" s="15" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="H32" s="27" t="s">
         <v>27</v>
@@ -3223,9 +3097,7 @@
       <c r="L32" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="M32" s="15" t="s">
-        <v>134</v>
-      </c>
+      <c r="M32" s="15"/>
       <c r="N32" s="27" t="s">
         <v>27</v>
       </c>
@@ -3245,7 +3117,7 @@
       <c r="E33" s="43"/>
       <c r="F33" s="43"/>
       <c r="G33" s="17" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="H33" s="29" t="s">
         <v>27</v>
@@ -3258,9 +3130,7 @@
       <c r="L33" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="M33" s="17" t="s">
-        <v>135</v>
-      </c>
+      <c r="M33" s="17"/>
       <c r="N33" s="29" t="s">
         <v>27</v>
       </c>
@@ -3288,7 +3158,7 @@
       </c>
       <c r="F34" s="41"/>
       <c r="G34" s="15" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="H34" s="27" t="s">
         <v>27</v>
@@ -3301,9 +3171,7 @@
       <c r="L34" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M34" s="15" t="s">
-        <v>136</v>
-      </c>
+      <c r="M34" s="15"/>
       <c r="N34" s="27" t="s">
         <v>27</v>
       </c>
@@ -3323,7 +3191,7 @@
       <c r="E35" s="42"/>
       <c r="F35" s="42"/>
       <c r="G35" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="H35" s="28" t="s">
         <v>27</v>
@@ -3336,9 +3204,7 @@
       <c r="L35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M35" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="M35" s="1"/>
       <c r="N35" s="28" t="s">
         <v>27</v>
       </c>
@@ -3358,7 +3224,7 @@
       <c r="E36" s="43"/>
       <c r="F36" s="43"/>
       <c r="G36" s="17" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="H36" s="29" t="s">
         <v>27</v>
@@ -3371,9 +3237,7 @@
       <c r="L36" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="M36" s="17" t="s">
-        <v>138</v>
-      </c>
+      <c r="M36" s="17"/>
       <c r="N36" s="29" t="s">
         <v>27</v>
       </c>
@@ -3387,14 +3251,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="44">
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="C34:C36"/>
     <mergeCell ref="D34:D36"/>
     <mergeCell ref="E34:E36"/>
-    <mergeCell ref="M16:R16"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:D33"/>
     <mergeCell ref="E32:E33"/>

</xml_diff>

<commit_message>
Export high-fidelity outcome03 desktop
</commit_message>
<xml_diff>
--- a/TrackList.xlsx
+++ b/TrackList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Team-Code_Life\mefado-ui-design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E884F5C9-5141-4639-A05B-09D9E825EE7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4B4D8C-A81D-4DF2-BEB1-95043B8531E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{279BB581-13DC-4C67-A208-ECEAEC5F3134}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="116">
   <si>
     <t>Outcomes</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>Xem DS các bài đăng (map view)</t>
+  </si>
+  <si>
+    <t>OUT03-01-D</t>
+  </si>
+  <si>
+    <t>OUT03-02-D</t>
   </si>
 </sst>
 </file>
@@ -768,15 +774,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -786,21 +801,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -838,12 +850,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1979,8 +1985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95DB2D2-227C-4DF4-891D-B90556287239}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2014,35 +2020,35 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="48" t="s">
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="48" t="s">
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="50"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="52"/>
       <c r="S2" s="1"/>
     </row>
     <row r="3" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="54"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
@@ -2094,19 +2100,19 @@
       <c r="S3" s="1"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="53"/>
+      <c r="F4" s="55"/>
       <c r="G4" s="9" t="s">
         <v>76</v>
       </c>
@@ -2132,11 +2138,11 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="59"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="52"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="54"/>
       <c r="G5" s="11" t="s">
         <v>77</v>
       </c>
@@ -2162,19 +2168,19 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="51"/>
+      <c r="F6" s="53"/>
       <c r="G6" s="13" t="s">
         <v>78</v>
       </c>
@@ -2200,11 +2206,11 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="59"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="52"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="54"/>
       <c r="G7" s="11" t="s">
         <v>79</v>
       </c>
@@ -2233,16 +2239,16 @@
       <c r="B8" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="15" t="s">
         <v>80</v>
       </c>
@@ -2255,12 +2261,16 @@
       <c r="L8" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="M8" s="13"/>
+      <c r="M8" s="15" t="s">
+        <v>114</v>
+      </c>
       <c r="N8" s="27"/>
       <c r="O8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="P8" s="27"/>
+      <c r="P8" s="27" t="s">
+        <v>108</v>
+      </c>
       <c r="Q8" s="27"/>
       <c r="R8" s="16" t="s">
         <v>62</v>
@@ -2268,10 +2278,10 @@
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="45"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="17" t="s">
         <v>81</v>
       </c>
@@ -2284,10 +2294,14 @@
       <c r="L9" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="M9" s="11"/>
+      <c r="M9" s="17" t="s">
+        <v>115</v>
+      </c>
       <c r="N9" s="29"/>
       <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
+      <c r="P9" s="29" t="s">
+        <v>108</v>
+      </c>
       <c r="Q9" s="29"/>
       <c r="R9" s="18" t="s">
         <v>63</v>
@@ -2297,16 +2311,16 @@
       <c r="B10" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="15" t="s">
         <v>82</v>
       </c>
@@ -2334,10 +2348,10 @@
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="45"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="17" t="s">
         <v>83</v>
       </c>
@@ -2395,19 +2409,19 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="41"/>
+      <c r="D13" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="35"/>
       <c r="G13" s="15" t="s">
         <v>85</v>
       </c>
@@ -2439,11 +2453,11 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="36"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
       <c r="G14" s="1" t="s">
         <v>86</v>
       </c>
@@ -2473,8 +2487,8 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="36"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="42"/>
       <c r="D15" s="6" t="s">
         <v>27</v>
       </c>
@@ -2512,8 +2526,8 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="36"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="42"/>
       <c r="D16" s="6" t="s">
         <v>27</v>
       </c>
@@ -2544,8 +2558,8 @@
       <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="36"/>
-      <c r="C17" s="39"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="42"/>
       <c r="D17" s="6" t="s">
         <v>27</v>
       </c>
@@ -2581,8 +2595,8 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="40"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="24" t="s">
         <v>27</v>
       </c>
@@ -2661,19 +2675,19 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="38"/>
+      <c r="D20" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="41"/>
       <c r="G20" s="15" t="s">
         <v>91</v>
       </c>
@@ -2703,11 +2717,11 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="39"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="42"/>
       <c r="G21" s="1" t="s">
         <v>92</v>
       </c>
@@ -2737,11 +2751,11 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="39"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="42"/>
       <c r="G22" s="1" t="s">
         <v>93</v>
       </c>
@@ -2771,11 +2785,11 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="1" t="s">
         <v>94</v>
       </c>
@@ -2805,11 +2819,11 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="36"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="39"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="42"/>
       <c r="G24" s="1" t="s">
         <v>95</v>
       </c>
@@ -2838,11 +2852,11 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="36"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="39"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="42"/>
       <c r="G25" s="1" t="s">
         <v>96</v>
       </c>
@@ -2872,11 +2886,11 @@
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="36"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="39"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="1" t="s">
         <v>97</v>
       </c>
@@ -2905,11 +2919,11 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="36"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="39"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="42"/>
       <c r="G27" s="1" t="s">
         <v>98</v>
       </c>
@@ -2938,11 +2952,11 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="36"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="39"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="42"/>
       <c r="G28" s="1" t="s">
         <v>99</v>
       </c>
@@ -2971,11 +2985,11 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="36"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="42"/>
       <c r="G29" s="1" t="s">
         <v>100</v>
       </c>
@@ -3004,11 +3018,11 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="36"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="42"/>
       <c r="G30" s="1" t="s">
         <v>101</v>
       </c>
@@ -3037,11 +3051,11 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="37"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="40"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="43"/>
       <c r="G31" s="17" t="s">
         <v>102</v>
       </c>
@@ -3070,19 +3084,19 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="41"/>
+      <c r="D32" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="35"/>
       <c r="G32" s="15" t="s">
         <v>103</v>
       </c>
@@ -3111,11 +3125,11 @@
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B33" s="37"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
       <c r="G33" s="17" t="s">
         <v>104</v>
       </c>
@@ -3144,19 +3158,19 @@
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" s="41"/>
+      <c r="D34" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="35"/>
       <c r="G34" s="15" t="s">
         <v>105</v>
       </c>
@@ -3185,11 +3199,11 @@
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B35" s="36"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="1" t="s">
         <v>106</v>
       </c>
@@ -3218,11 +3232,11 @@
       </c>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B36" s="37"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
       <c r="G36" s="17" t="s">
         <v>107</v>
       </c>
@@ -3252,22 +3266,13 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F20:F31"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D20:D31"/>
+    <mergeCell ref="E20:E31"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="B13:B18"/>
     <mergeCell ref="M2:R2"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="F4:F5"/>
@@ -3279,6 +3284,12 @@
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="G2:L2"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F20:F31"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="F13:F14"/>
@@ -3289,13 +3300,16 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="B20:B31"/>
     <mergeCell ref="C20:C31"/>
-    <mergeCell ref="D20:D31"/>
-    <mergeCell ref="E20:E31"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="B13:B18"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>